<commit_message>
collected data for duck puzzle
</commit_message>
<xml_diff>
--- a/a1.xlsx
+++ b/a1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CurtisLui/Documents/Documents/SFU /4th Year/SUMMER 2020/CMPT 310/aima-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCB8934-AAA3-984A-8196-ED4EC7C67F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BFDBD7-F5A5-3F47-A53F-9857EB72015F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{423D17DF-81E2-8D47-A949-B41332F7DC77}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="37900" windowHeight="21140" xr2:uid="{423D17DF-81E2-8D47-A949-B41332F7DC77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>(7, 4, 1, 0, 3, 2, 8, 5, 6)</t>
   </si>
@@ -84,18 +84,6 @@
     <t>(3, 1, 8, 0, 2, 6, 7, 5, 4)</t>
   </si>
   <si>
-    <t>misplaced heuristic is a large underestimation</t>
-  </si>
-  <si>
-    <t>set of actions are different</t>
-  </si>
-  <si>
-    <t>duck puzzle:</t>
-  </si>
-  <si>
-    <t>result will be different</t>
-  </si>
-  <si>
     <t>Question 2: Comparing Algorithms</t>
   </si>
   <si>
@@ -127,6 +115,39 @@
   </si>
   <si>
     <t>Comparing Duck-Puzzle to 8-Puzzle</t>
+  </si>
+  <si>
+    <t>(3, 1, 2, 5, 4, 6, 0, 8, 7)</t>
+  </si>
+  <si>
+    <t>(1, 2, 3, 8, 0, 6, 5, 7, 4)</t>
+  </si>
+  <si>
+    <t>(1, 2, 0, 3, 6, 8, 4, 7, 5)</t>
+  </si>
+  <si>
+    <t>(2, 3, 1, 4, 8, 7, 6, 5, 0)</t>
+  </si>
+  <si>
+    <t>(3, 1, 2, 6, 0, 5, 8, 7, 4)</t>
+  </si>
+  <si>
+    <t>(1, 2, 3, 7, 8, 6, 4, 5, 0)</t>
+  </si>
+  <si>
+    <t>(3, 0, 2, 1, 5, 6, 8, 4, 7)</t>
+  </si>
+  <si>
+    <t>(2, 3, 1, 8, 0, 7, 5, 4, 6)</t>
+  </si>
+  <si>
+    <t>(2, 3, 1, 8, 5, 6, 0, 4, 7)</t>
+  </si>
+  <si>
+    <t>(3, 1, 2, 7, 5, 8, 4, 6, 0)</t>
+  </si>
+  <si>
+    <t>(3, 1, 2, 6, 0, 4, 5, 7, 8)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -244,39 +265,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -300,6 +337,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72999274-A13A-4147-AA55-324BBD695605}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,54 +698,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="A1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="11"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="L2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -692,13 +757,13 @@
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="L3" s="1"/>
@@ -706,34 +771,34 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="12">
         <v>3.7631988525390599E-3</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="11">
         <v>14</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="13">
         <v>83</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="11">
         <v>6.1702728271484299E-4</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="11">
         <v>14</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="11">
         <v>15</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="12">
         <v>4.4512748718261702E-4</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="11">
         <v>14</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="13">
         <v>15</v>
       </c>
       <c r="L4" s="1"/>
@@ -741,34 +806,34 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="9">
         <v>0.45156216621398898</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>19</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="10">
         <v>1286</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>4.4016838073730399E-2</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="6">
         <v>19</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="6">
         <v>342</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="9">
         <v>4.3816089630126898E-2</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="6">
         <v>19</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="10">
         <v>342</v>
       </c>
       <c r="L5" s="1"/>
@@ -776,34 +841,34 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="9">
         <v>516.83531188964798</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>27</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="10">
         <v>38363</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>2.3462421894073402</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="6">
         <v>27</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="6">
         <v>2972</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="9">
         <v>2.3777329921722399</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="6">
         <v>27</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="10">
         <v>2972</v>
       </c>
       <c r="L6" s="1"/>
@@ -811,34 +876,34 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="9">
         <v>5.5968999862670898E-2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>17</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="10">
         <v>396</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>4.4620037078857396E-3</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="6">
         <v>17</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="6">
         <v>89</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="9">
         <v>4.2881965637206997E-3</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="6">
         <v>17</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="10">
         <v>89</v>
       </c>
       <c r="L7" s="1"/>
@@ -846,34 +911,34 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="9">
         <v>22.224617004394499</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>24</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="10">
         <v>9326</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="6">
         <v>6.2270164489745997E-2</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <v>24</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="6">
         <v>420</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="9">
         <v>5.9733867645263602E-2</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="6">
         <v>24</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="10">
         <v>420</v>
       </c>
       <c r="L8" s="1"/>
@@ -881,34 +946,34 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="9">
         <v>43.950897932052598</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="6">
         <v>25</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="10">
         <v>12887</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="6">
         <v>0.15557885169982899</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="6">
         <v>25</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="6">
         <v>695</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="9">
         <v>0.15943694114685</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="6">
         <v>25</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="10">
         <v>695</v>
       </c>
       <c r="L9" s="1"/>
@@ -916,34 +981,34 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="9">
         <v>458.778995037078</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="6">
         <v>27</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="10">
         <v>34688</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="6">
         <v>1.12128210067749</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="6">
         <v>27</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="6">
         <v>2013</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="9">
         <v>1.12520503997802</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="6">
         <v>27</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="10">
         <v>2013</v>
       </c>
       <c r="L10" s="1"/>
@@ -951,34 +1016,34 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="9">
         <v>21.3444180488586</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>24</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="10">
         <v>9187</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="6">
         <v>5.0786733627319301E-2</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="6">
         <v>24</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="6">
         <v>366</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="9">
         <v>4.8313140869140597E-2</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="6">
         <v>24</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="10">
         <v>366</v>
       </c>
       <c r="L11" s="1"/>
@@ -986,34 +1051,34 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="9">
         <v>9.0247869491577095</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="6">
         <v>23</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="10">
         <v>5826</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="6">
         <v>7.4630260467529297E-2</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="6">
         <v>23</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="6">
         <v>467</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="9">
         <v>7.41009712219238E-2</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="6">
         <v>23</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="10">
         <v>467</v>
       </c>
       <c r="L12" s="1"/>
@@ -1021,34 +1086,34 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="9">
         <v>4.5554559230804399</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="6">
         <v>22</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="10">
         <v>4133</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="6">
         <v>3.2054901123046799E-2</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="6">
         <v>22</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="6">
         <v>282</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="9">
         <v>3.1358003616333001E-2</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="6">
         <v>22</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="10">
         <v>282</v>
       </c>
       <c r="L13" s="1"/>
@@ -1056,34 +1121,34 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="9">
         <v>4.4608860015869096</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="6">
         <v>22</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="10">
         <v>4093</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="6">
         <v>3.9394140243530197E-2</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="6">
         <v>22</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="6">
         <v>312</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="9">
         <v>3.9665937423705999E-2</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="6">
         <v>22</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="10">
         <v>312</v>
       </c>
       <c r="L14" s="1"/>
@@ -1091,46 +1156,46 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="3" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="10" t="s">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="11"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1142,283 +1207,834 @@
       <c r="G17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="17">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="12">
         <f>MIN(B4:B14)</f>
         <v>3.7631988525390599E-3</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="11">
         <f>MIN(C4:C14)</f>
         <v>14</v>
       </c>
-      <c r="D18" s="18">
-        <f t="shared" ref="C18:J18" si="0">MIN(D4:D14)</f>
+      <c r="D18" s="13">
+        <f t="shared" ref="D18:J18" si="0">MIN(D4:D14)</f>
         <v>83</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="11">
         <f t="shared" si="0"/>
         <v>6.1702728271484299E-4</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="11">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="12">
         <f t="shared" si="0"/>
         <v>4.4512748718261702E-4</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="13">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="14">
+      <c r="A19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="9">
         <f>MAX(B4:B14)</f>
         <v>516.83531188964798</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="6">
         <f t="shared" ref="C19:J19" si="1">MAX(C4:C14)</f>
         <v>27</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="10">
         <f t="shared" si="1"/>
         <v>38363</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="6">
         <f t="shared" si="1"/>
         <v>2.3462421894073402</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="6">
         <f t="shared" si="1"/>
         <v>2972</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="9">
         <f t="shared" si="1"/>
         <v>2.3777329921722399</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="10">
         <f t="shared" si="1"/>
         <v>2972</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="14">
+      <c r="A20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="9">
         <f>AVERAGE(B4:B14)</f>
         <v>98.335151195525995</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="6">
         <f t="shared" ref="C20:J20" si="2">AVERAGE(C4:C14)</f>
         <v>22.181818181818183</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="10">
         <f t="shared" si="2"/>
         <v>10933.454545454546</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="6">
         <f t="shared" si="2"/>
         <v>0.35739411007274202</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="6">
         <f t="shared" si="2"/>
         <v>22.181818181818183</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="6">
         <f t="shared" si="2"/>
         <v>724.81818181818187</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="9">
         <f t="shared" si="2"/>
         <v>0.36037239161404616</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="6">
         <f t="shared" si="2"/>
         <v>22.181818181818183</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="10">
         <f t="shared" si="2"/>
         <v>724.81818181818187</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="14">
+      <c r="A21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="9">
         <f>MEDIAN(B4:B14)</f>
         <v>9.0247869491577095</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="6">
         <f t="shared" ref="C21:J21" si="3">MEDIAN(C4:C14)</f>
         <v>23</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="10">
         <f t="shared" si="3"/>
         <v>5826</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="6">
         <f t="shared" si="3"/>
         <v>5.0786733627319301E-2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="6">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="6">
         <f t="shared" si="3"/>
         <v>366</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="9">
         <f t="shared" si="3"/>
         <v>4.8313140869140597E-2</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="6">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="10">
         <f t="shared" si="3"/>
         <v>366</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="18"/>
+      <c r="L24" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+    </row>
+    <row r="25" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="L24" s="3" t="s">
+      <c r="B26" s="22">
+        <v>1.6665935516357401E-2</v>
+      </c>
+      <c r="C26" s="23">
+        <v>19</v>
+      </c>
+      <c r="D26" s="24">
+        <v>284</v>
+      </c>
+      <c r="E26">
+        <v>6.7546367645263602E-3</v>
+      </c>
+      <c r="F26">
+        <v>19</v>
+      </c>
+      <c r="G26">
+        <v>121</v>
+      </c>
+      <c r="H26" s="22">
+        <v>5.1600933074951102E-3</v>
+      </c>
+      <c r="I26" s="23">
+        <v>19</v>
+      </c>
+      <c r="J26" s="24">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="22">
+        <v>9.8769664764404297E-3</v>
+      </c>
+      <c r="C27" s="23">
+        <v>15</v>
+      </c>
+      <c r="D27" s="24">
+        <v>164</v>
+      </c>
+      <c r="E27">
+        <v>4.55594062805175E-3</v>
+      </c>
+      <c r="F27">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>65</v>
+      </c>
+      <c r="H27" s="25">
+        <v>2.3121833801269501E-3</v>
+      </c>
+      <c r="I27" s="23">
+        <v>15</v>
+      </c>
+      <c r="J27" s="24">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="22">
+        <v>3.18050384521484E-4</v>
+      </c>
+      <c r="C28" s="23">
+        <v>9</v>
+      </c>
+      <c r="D28" s="24">
+        <v>13</v>
+      </c>
+      <c r="E28">
+        <v>2.3221969604492101E-4</v>
+      </c>
+      <c r="F28">
+        <v>9</v>
+      </c>
+      <c r="G28">
+        <v>9</v>
+      </c>
+      <c r="H28" s="22">
+        <v>2.2912025451660099E-4</v>
+      </c>
+      <c r="I28" s="23">
+        <v>9</v>
+      </c>
+      <c r="J28" s="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>4</v>
+      <c r="B29" s="22">
+        <v>2.6054859161376901E-2</v>
+      </c>
+      <c r="C29" s="23">
+        <v>19</v>
+      </c>
+      <c r="D29" s="24">
+        <v>281</v>
+      </c>
+      <c r="E29">
+        <v>2.3977756500244102E-3</v>
+      </c>
+      <c r="F29">
+        <v>19</v>
+      </c>
+      <c r="G29">
+        <v>67</v>
+      </c>
+      <c r="H29" s="22">
+        <v>2.19488143920898E-3</v>
+      </c>
+      <c r="I29" s="23">
+        <v>19</v>
+      </c>
+      <c r="J29" s="24">
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="B30" s="22">
+        <v>9.7701311111450195E-2</v>
+      </c>
+      <c r="C30" s="23">
+        <v>23</v>
+      </c>
+      <c r="D30" s="24">
+        <v>797</v>
+      </c>
+      <c r="E30">
+        <v>2.9439926147460899E-2</v>
+      </c>
+      <c r="F30">
+        <v>23</v>
+      </c>
+      <c r="G30">
+        <v>363</v>
+      </c>
+      <c r="H30" s="22">
+        <v>3.2855033874511698E-2</v>
+      </c>
+      <c r="I30" s="23">
+        <v>23</v>
+      </c>
+      <c r="J30" s="24">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="22">
+        <v>6.4600944519042899E-2</v>
+      </c>
+      <c r="C31" s="23">
+        <v>21</v>
+      </c>
+      <c r="D31" s="24">
+        <v>553</v>
+      </c>
+      <c r="E31">
+        <v>2.5180816650390601E-2</v>
+      </c>
+      <c r="F31">
+        <v>21</v>
+      </c>
+      <c r="G31">
+        <v>310</v>
+      </c>
+      <c r="H31" s="22">
+        <v>2.7255058288574201E-2</v>
+      </c>
+      <c r="I31" s="23">
+        <v>21</v>
+      </c>
+      <c r="J31" s="24">
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="22">
+        <v>8.5330009460449201E-3</v>
+      </c>
+      <c r="C32" s="23">
+        <v>17</v>
+      </c>
+      <c r="D32" s="24">
+        <v>154</v>
+      </c>
+      <c r="E32">
+        <v>2.9058456420898398E-3</v>
+      </c>
+      <c r="F32">
+        <v>17</v>
+      </c>
+      <c r="G32">
+        <v>70</v>
+      </c>
+      <c r="H32" s="22">
+        <v>2.5219917297363199E-3</v>
+      </c>
+      <c r="I32" s="23">
+        <v>17</v>
+      </c>
+      <c r="J32" s="24">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="22">
+        <v>1.49381160736083E-2</v>
+      </c>
+      <c r="C33" s="23">
+        <v>17</v>
+      </c>
+      <c r="D33" s="24">
+        <v>202</v>
+      </c>
+      <c r="E33">
+        <v>1.81818008422851E-3</v>
+      </c>
+      <c r="F33">
+        <v>17</v>
+      </c>
+      <c r="G33">
+        <v>54</v>
+      </c>
+      <c r="H33" s="22">
+        <v>2.1460056304931602E-3</v>
+      </c>
+      <c r="I33" s="23">
+        <v>17</v>
+      </c>
+      <c r="J33" s="24">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="22">
+        <v>5.8259963989257804E-3</v>
+      </c>
+      <c r="C34" s="23">
+        <v>15</v>
+      </c>
+      <c r="D34" s="24">
+        <v>97</v>
+      </c>
+      <c r="E34">
+        <v>4.3678283691406198E-3</v>
+      </c>
+      <c r="F34">
+        <v>15</v>
+      </c>
+      <c r="G34">
+        <v>62</v>
+      </c>
+      <c r="H34" s="22">
+        <v>1.9640922546386701E-3</v>
+      </c>
+      <c r="I34" s="23">
+        <v>15</v>
+      </c>
+      <c r="J34" s="24">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="22">
+        <v>0.141741037368774</v>
+      </c>
+      <c r="C35" s="23">
+        <v>25</v>
+      </c>
+      <c r="D35" s="24">
+        <v>1011</v>
+      </c>
+      <c r="E35">
+        <v>5.2363634109497001E-2</v>
+      </c>
+      <c r="F35">
+        <v>25</v>
+      </c>
+      <c r="G35">
+        <v>521</v>
+      </c>
+      <c r="H35" s="22">
+        <v>5.5527925491333001E-2</v>
+      </c>
+      <c r="I35" s="23">
+        <v>25</v>
+      </c>
+      <c r="J35" s="24">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="22">
+        <v>3.5205841064453097E-2</v>
+      </c>
+      <c r="C36" s="23">
         <v>19</v>
       </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+      <c r="D36" s="24">
+        <v>345</v>
+      </c>
+      <c r="E36">
+        <v>7.8949928283691406E-3</v>
+      </c>
+      <c r="F36">
+        <v>19</v>
+      </c>
+      <c r="G36">
+        <v>161</v>
+      </c>
+      <c r="H36" s="23">
+        <v>8.0909729003906198E-3</v>
+      </c>
+      <c r="I36" s="23">
+        <v>19</v>
+      </c>
+      <c r="J36" s="23">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" s="17"/>
+      <c r="J38" s="18"/>
+    </row>
+    <row r="39" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="12">
+        <f>MIN(B26:B36)</f>
+        <v>3.18050384521484E-4</v>
+      </c>
+      <c r="C40" s="11">
+        <f>MIN(C26:C36)</f>
+        <v>9</v>
+      </c>
+      <c r="D40" s="13">
+        <f t="shared" ref="D40:J40" si="4">MIN(D26:D36)</f>
+        <v>13</v>
+      </c>
+      <c r="E40" s="11">
+        <f t="shared" si="4"/>
+        <v>2.3221969604492101E-4</v>
+      </c>
+      <c r="F40" s="11">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="G40" s="11">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H40" s="12">
+        <f t="shared" si="4"/>
+        <v>2.2912025451660099E-4</v>
+      </c>
+      <c r="I40" s="11">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="J40" s="13">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="B41" s="9">
+        <f>MAX(B26:B36)</f>
+        <v>0.141741037368774</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" ref="C41:J41" si="5">MAX(C26:C36)</f>
+        <v>25</v>
+      </c>
+      <c r="D41" s="10">
+        <f t="shared" si="5"/>
+        <v>1011</v>
+      </c>
+      <c r="E41" s="6">
+        <f t="shared" si="5"/>
+        <v>5.2363634109497001E-2</v>
+      </c>
+      <c r="F41" s="6">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="G41" s="6">
+        <f t="shared" si="5"/>
+        <v>521</v>
+      </c>
+      <c r="H41" s="9">
+        <f t="shared" si="5"/>
+        <v>5.5527925491333001E-2</v>
+      </c>
+      <c r="I41" s="6">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="5"/>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="9">
+        <f>AVERAGE(B26:B36)</f>
+        <v>3.8314732638272314E-2</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" ref="C42:J42" si="6">AVERAGE(C26:C36)</f>
+        <v>18.09090909090909</v>
+      </c>
+      <c r="D42" s="10">
+        <f t="shared" si="6"/>
+        <v>354.63636363636363</v>
+      </c>
+      <c r="E42" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2537436051802187E-2</v>
+      </c>
+      <c r="F42" s="6">
+        <f t="shared" si="6"/>
+        <v>18.09090909090909</v>
+      </c>
+      <c r="G42" s="6">
+        <f t="shared" si="6"/>
+        <v>163.90909090909091</v>
+      </c>
+      <c r="H42" s="9">
+        <f t="shared" si="6"/>
+        <v>1.2750668959184119E-2</v>
+      </c>
+      <c r="I42" s="6">
+        <f t="shared" si="6"/>
+        <v>18.09090909090909</v>
+      </c>
+      <c r="J42" s="10">
+        <f t="shared" si="6"/>
+        <v>163.90909090909091</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="9">
+        <f>MEDIAN(B26:B36)</f>
+        <v>1.6665935516357401E-2</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" ref="C43:J43" si="7">MEDIAN(C26:C36)</f>
+        <v>19</v>
+      </c>
+      <c r="D43" s="10">
+        <f t="shared" si="7"/>
+        <v>281</v>
+      </c>
+      <c r="E43" s="6">
+        <f t="shared" si="7"/>
+        <v>4.55594062805175E-3</v>
+      </c>
+      <c r="F43" s="6">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="G43" s="6">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="H43" s="9">
+        <f t="shared" si="7"/>
+        <v>2.5219917297363199E-3</v>
+      </c>
+      <c r="I43" s="6">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="J43" s="10">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="L24:N24"/>
     <mergeCell ref="A23:J23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="H24:J24"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>